<commit_message>
1) Added Email Message content
2) Added Unit Test cases
</commit_message>
<xml_diff>
--- a/Project Matrix.xlsx
+++ b/Project Matrix.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Accounts creation" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Java Version </t>
   </si>
   <si>
     <t>Java SE 1.7</t>
+  </si>
+  <si>
+    <t>C:\informatica\Customer\Customer Screenshots\Customer BCBS Screenshot 2014-07-19 21_14_56.png</t>
   </si>
 </sst>
 </file>
@@ -160,6 +163,55 @@
         <a:xfrm>
           <a:off x="0" y="8382000"/>
           <a:ext cx="18285716" cy="10285715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="5657850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -460,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,11 +540,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>